<commit_message>
organized the model_shift_matrices and changed parameters, final version
</commit_message>
<xml_diff>
--- a/Emissions/emission_factors/CO2e/Modal_Shift_Matrix.xlsx
+++ b/Emissions/emission_factors/CO2e/Modal_Shift_Matrix.xlsx
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E2" t="n">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -523,19 +523,19 @@
         <v>66</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the formula for CO2e and add individual graphs, final commit
</commit_message>
<xml_diff>
--- a/Emissions/emission_factors/CO2e/Modal_Shift_Matrix.xlsx
+++ b/Emissions/emission_factors/CO2e/Modal_Shift_Matrix.xlsx
@@ -529,13 +529,13 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L2" t="n">
         <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>